<commit_message>
fechando chamada + salvando via .json
</commit_message>
<xml_diff>
--- a/data/logPiscina.xlsx
+++ b/data/logPiscina.xlsx
@@ -1,43 +1,136 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Lista-de-Chamada-Web\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446C89FE-C904-4620-B61C-1F9E233AB08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Clima 1</t>
+  </si>
+  <si>
+    <t>Clima 2</t>
+  </si>
+  <si>
+    <t>Status_aula</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>Tipo_ocorrencia</t>
+  </si>
+  <si>
+    <t>Temp. (C)</t>
+  </si>
+  <si>
+    <t>Piscina (C)</t>
+  </si>
+  <si>
+    <t>Cloro (ppm)</t>
+  </si>
+  <si>
+    <t>TurmaCodigo</t>
+  </si>
+  <si>
+    <t>TurmaLabel</t>
+  </si>
+  <si>
+    <t>Horario</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>2026-02-04</t>
+  </si>
+  <si>
+    <t>Nublado</t>
+  </si>
+  <si>
+    <t>Vento</t>
+  </si>
+  <si>
+    <t>justificada</t>
+  </si>
+  <si>
+    <t>aula</t>
+  </si>
+  <si>
+    <t>nenhuma</t>
+  </si>
+  <si>
+    <t>jqs01</t>
+  </si>
+  <si>
+    <t>Quarta e Sexta</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>Jefferson</t>
+  </si>
+  <si>
+    <t>Agradavel</t>
+  </si>
+  <si>
+    <t>2026-02-06</t>
+  </si>
+  <si>
+    <t>Sol</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,94 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,109 +445,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Data</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Clima 1</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Clima 2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Status_aula</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Nota</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo_ocorrencia</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Temp. (C)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Piscina (C)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Cloro (ppm)</t>
-        </is>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2026-02-03</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Parcialmente Nublado</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Agradavel</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>aula</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nenhuma</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>30.5</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>1.5</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>26</v>
+      </c>
+      <c r="H2">
+        <v>31</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza chamada e clima de fev/2026, integra hidratação no frontend e ajusta ordenação de horários
</commit_message>
<xml_diff>
--- a/data/logPiscina.xlsx
+++ b/data/logPiscina.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,17 +496,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nublado</t>
+          <t>Parcialmente Nublado</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vento</t>
+          <t>Agradavel</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>justificada</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -514,40 +514,18 @@
           <t>aula</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nenhuma</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
-        <v>26</v>
-      </c>
-      <c r="H2" t="n">
         <v>31</v>
       </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
         <v>6</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>jqs01</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Quarta e Sexta</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Jefferson</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -575,40 +553,18 @@
           <t>aula</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nenhuma</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
-        <v>26</v>
-      </c>
-      <c r="H3" t="n">
-        <v>32</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>4</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>jqs01</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Quarta e Sexta</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Jefferson</t>
-        </is>
-      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -618,17 +574,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nublado</t>
+          <t>Parcialmente Nublado</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Vento</t>
+          <t>Agradavel</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>justificada</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -636,40 +592,18 @@
           <t>aula</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nenhuma</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
-        <v>26</v>
-      </c>
-      <c r="H4" t="n">
         <v>31</v>
       </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>6</v>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>dqs02</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Quarta e Sexta</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>10:15</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Daniela</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -697,40 +631,18 @@
           <t>aula</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nenhuma</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>26</v>
-      </c>
-      <c r="H5" t="n">
-        <v>32</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>4</v>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>dqs02</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Quarta e Sexta</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>10:15</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Daniela</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -740,17 +652,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nublado</t>
+          <t>Parcialmente Nublado</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Vento</t>
+          <t>Agradavel</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>justificada</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -758,44 +670,407 @@
           <t>aula</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nenhuma</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>31</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
         <v>6</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>dqs03</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Quarta e Sexta</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Daniela</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>cancelada</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ponte-feriado</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>cancelada</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ponte-feriado</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>cancelada</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ponte-feriado</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>cancelada</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ponte-feriado</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Agradavel</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>aula</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>32</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>6</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Sol</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Agradavel</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>aula</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>31</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Chuvoso</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Frio</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>aula</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>29</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>3</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Parcialmente Nublado</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Calor</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>aula</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>29</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>cancelada</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>feriado</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Chuvoso</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Frio</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>aula</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>29</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>3</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Parcialmente Nublado</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Calor</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>aula</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
+        <v>29</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: integrar regras de calendario na chamada e progresso anual de dias previstos
</commit_message>
<xml_diff>
--- a/data/logPiscina.xlsx
+++ b/data/logPiscina.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1072,6 +1072,69 @@
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Agradavel</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>cancelada</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>reuniao</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>nenhuma</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>26.0</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>jtq07</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Terça e Quinta</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>15:15</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Jefferson</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
antes de duploclick em chamada
</commit_message>
<xml_diff>
--- a/data/logPiscina.xlsx
+++ b/data/logPiscina.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,10 +1103,8 @@
           <t>nenhuma</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>26.0</t>
-        </is>
+      <c r="G18" t="n">
+        <v>26</v>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
@@ -1132,6 +1130,71 @@
       <c r="M18" t="inlineStr">
         <is>
           <t>Jefferson</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Sol</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Agradavel</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>aula</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>nenhuma</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>dqs01</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Quarta e Sexta</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Daniela</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(frontend): add partial value labels to stacked bar chart segments in DashboardCharts
- Added occurrence-segment-label that displays present/absent/justified counts
- Only show labels when segment width > 8% to avoid text overflow
- Used small font size (10px) with white color and text-shadow for readability
- Styled segments as flex containers for proper label centering
- Improves data visualization in 'Registros por turma' chart
</commit_message>
<xml_diff>
--- a/data/logPiscina.xlsx
+++ b/data/logPiscina.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Lista-de-Chamada-Web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671028FF-87E8-478A-BB22-0718833F9282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8551DED2-50B4-45C7-8283-945C030A6B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -506,7 +509,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,10 +560,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -572,7 +575,7 @@
         <v>17</v>
       </c>
       <c r="G2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I2">
         <v>6</v>
@@ -580,10 +583,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -595,10 +598,10 @@
         <v>17</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -626,10 +629,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -641,18 +644,18 @@
         <v>17</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -667,74 +670,110 @@
         <v>31</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>29</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="G10">
+        <v>29</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -743,21 +782,21 @@
         <v>17</v>
       </c>
       <c r="G11">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
@@ -766,67 +805,49 @@
         <v>17</v>
       </c>
       <c r="G12">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13">
-        <v>29</v>
-      </c>
-      <c r="I13">
-        <v>3</v>
+        <v>33</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14">
-        <v>29</v>
-      </c>
-      <c r="I14">
-        <v>2.5</v>
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I15" t="s">
         <v>23</v>
@@ -834,53 +855,35 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16">
-        <v>29</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17">
-        <v>29</v>
-      </c>
-      <c r="I17">
-        <v>2.5</v>
+        <v>22</v>
+      </c>
+      <c r="I17" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -901,22 +904,22 @@
         <v>27</v>
       </c>
       <c r="H18">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="J18" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="L18" t="s">
         <v>43</v>
       </c>
       <c r="M18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -939,22 +942,22 @@
         <v>37</v>
       </c>
       <c r="G19">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19">
-        <v>31</v>
+        <v>32.5</v>
       </c>
       <c r="I19">
         <v>1.5</v>
       </c>
       <c r="J19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K19" t="s">
         <v>38</v>
       </c>
       <c r="L19" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M19" t="s">
         <v>39</v>
@@ -962,7 +965,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -980,28 +983,33 @@
         <v>37</v>
       </c>
       <c r="G20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H20">
-        <v>32.5</v>
+        <v>32</v>
       </c>
       <c r="I20">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="J20" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="L20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M20" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M20">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore(data): update attendance base files and pool log
</commit_message>
<xml_diff>
--- a/data/logPiscina.xlsx
+++ b/data/logPiscina.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1377,6 +1377,67 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Parcialmente Nublado</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Abafado</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>aula</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>nenhuma</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>jtq01</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Terça e Quinta</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Jefferson</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>